<commit_message>
Descripción de los cambios, Correccion de precios.
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -1185,7 +1185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1223,8 +1223,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1255,8 +1262,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1277,12 +1290,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1313,6 +1341,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1357,7 +1386,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:G131" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:G131"/>
+  <autoFilter ref="A1:G131">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Tenis Plataforma Hombre Air Original Tendencia Alta Hip Hop"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:G131">
     <sortCondition ref="G1:G131"/>
   </sortState>
@@ -1639,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,7 +1711,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>307</v>
       </c>
@@ -1699,7 +1734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>302</v>
       </c>
@@ -1722,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>299</v>
       </c>
@@ -1745,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>296</v>
       </c>
@@ -1765,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>377</v>
       </c>
@@ -1788,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>290</v>
       </c>
@@ -1811,7 +1846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>289</v>
       </c>
@@ -1834,7 +1869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>287</v>
       </c>
@@ -1854,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>283</v>
       </c>
@@ -1877,7 +1912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -1900,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>277</v>
       </c>
@@ -1923,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>274</v>
       </c>
@@ -1946,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>270</v>
       </c>
@@ -1969,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>267</v>
       </c>
@@ -1992,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>264</v>
       </c>
@@ -2015,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>382</v>
       </c>
@@ -2038,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>259</v>
       </c>
@@ -2061,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>258</v>
       </c>
@@ -2084,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>253</v>
       </c>
@@ -2107,7 +2142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>250</v>
       </c>
@@ -2127,7 +2162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -2154,8 +2189,8 @@
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B23" t="s">
-        <v>204</v>
+      <c r="B23" s="18" t="s">
+        <v>376</v>
       </c>
       <c r="C23" s="3">
         <v>419.19</v>
@@ -2173,7 +2208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2193,7 +2228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2213,7 +2248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>308</v>
       </c>
@@ -2233,7 +2268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>309</v>
       </c>
@@ -2256,7 +2291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2279,7 +2314,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>373</v>
       </c>
@@ -2302,7 +2337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -2322,7 +2357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>313</v>
       </c>
@@ -2345,7 +2380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>312</v>
       </c>
@@ -2368,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2388,7 +2423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2408,7 +2443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>310</v>
       </c>
@@ -2428,7 +2463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -2448,7 +2483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2468,7 +2503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>316</v>
       </c>
@@ -2491,7 +2526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>323</v>
       </c>
@@ -2514,7 +2549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>371</v>
       </c>
@@ -2535,7 +2570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>361</v>
       </c>
@@ -2558,7 +2593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>364</v>
       </c>
@@ -2581,7 +2616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>367</v>
       </c>
@@ -2604,7 +2639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>370</v>
       </c>
@@ -2625,7 +2660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
         <v>357</v>
       </c>
@@ -2646,7 +2681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
         <v>358</v>
       </c>
@@ -2667,7 +2702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>329</v>
       </c>
@@ -2690,7 +2725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
         <v>349</v>
       </c>
@@ -2711,7 +2746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
         <v>352</v>
       </c>
@@ -2732,7 +2767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
         <v>332</v>
       </c>
@@ -2755,7 +2790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
         <v>335</v>
       </c>
@@ -2778,7 +2813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
         <v>338</v>
       </c>
@@ -2801,7 +2836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>340</v>
       </c>
@@ -2822,7 +2857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
         <v>342</v>
       </c>
@@ -2845,7 +2880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>347</v>
       </c>
@@ -2866,7 +2901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>345</v>
       </c>
@@ -2887,7 +2922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>326</v>
       </c>
@@ -2910,7 +2945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -2933,7 +2968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2956,7 +2991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -2979,7 +3014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -3002,7 +3037,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3025,7 +3060,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -3045,7 +3080,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>13</v>
       </c>
@@ -3062,7 +3097,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>14</v>
       </c>
@@ -3085,7 +3120,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -3108,7 +3143,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -3131,7 +3166,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -3154,7 +3189,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -3177,7 +3212,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -3200,7 +3235,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>20</v>
       </c>
@@ -3220,7 +3255,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>21</v>
       </c>
@@ -3240,7 +3275,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>383</v>
       </c>
@@ -3263,7 +3298,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>22</v>
       </c>
@@ -3283,7 +3318,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>378</v>
       </c>
@@ -3306,7 +3341,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>23</v>
       </c>
@@ -3326,7 +3361,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>24</v>
       </c>
@@ -3346,7 +3381,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>25</v>
       </c>
@@ -3369,7 +3404,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>26</v>
       </c>
@@ -3392,7 +3427,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>27</v>
       </c>
@@ -3415,7 +3450,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>28</v>
       </c>
@@ -3438,7 +3473,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>29</v>
       </c>
@@ -3461,7 +3496,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>35</v>
       </c>
@@ -3484,7 +3519,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>36</v>
       </c>
@@ -3507,7 +3542,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>37</v>
       </c>
@@ -3530,7 +3565,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>38</v>
       </c>
@@ -3553,7 +3588,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>322</v>
       </c>
@@ -3576,7 +3611,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -3599,7 +3634,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>40</v>
       </c>
@@ -3622,7 +3657,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>41</v>
       </c>
@@ -3642,7 +3677,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -3662,7 +3697,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>43</v>
       </c>
@@ -3685,7 +3720,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>44</v>
       </c>
@@ -3708,7 +3743,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>45</v>
       </c>
@@ -3731,7 +3766,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>46</v>
       </c>
@@ -3754,7 +3789,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -3777,7 +3812,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -3800,7 +3835,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>49</v>
       </c>
@@ -3820,7 +3855,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>50</v>
       </c>
@@ -3843,7 +3878,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>51</v>
       </c>
@@ -3866,7 +3901,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>52</v>
       </c>
@@ -3886,7 +3921,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>53</v>
       </c>
@@ -3906,7 +3941,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>54</v>
       </c>
@@ -3929,7 +3964,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>55</v>
       </c>
@@ -3952,7 +3987,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>56</v>
       </c>
@@ -3975,7 +4010,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>57</v>
       </c>
@@ -3995,7 +4030,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>58</v>
       </c>
@@ -4018,7 +4053,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>381</v>
       </c>
@@ -4035,7 +4070,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>59</v>
       </c>
@@ -4058,7 +4093,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>60</v>
       </c>
@@ -4078,7 +4113,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>61</v>
       </c>
@@ -4098,7 +4133,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>62</v>
       </c>
@@ -4115,7 +4150,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>63</v>
       </c>
@@ -4132,7 +4167,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>64</v>
       </c>
@@ -4155,7 +4190,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>65</v>
       </c>
@@ -4178,7 +4213,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>66</v>
       </c>
@@ -4201,7 +4236,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>67</v>
       </c>
@@ -4221,7 +4256,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>69</v>
       </c>
@@ -4244,7 +4279,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>380</v>
       </c>
@@ -4264,7 +4299,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>70</v>
       </c>
@@ -4287,7 +4322,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>243</v>
       </c>
@@ -4308,7 +4343,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>71</v>
       </c>
@@ -4328,7 +4363,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>379</v>
       </c>
@@ -4348,7 +4383,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>72</v>
       </c>
@@ -4368,7 +4403,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>73</v>
       </c>
@@ -4391,7 +4426,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>75</v>
       </c>
@@ -4414,7 +4449,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>76</v>
       </c>
@@ -4437,7 +4472,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>77</v>
       </c>
@@ -4457,7 +4492,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>78</v>
       </c>
@@ -4480,7 +4515,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>80</v>
       </c>
@@ -4503,7 +4538,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>320</v>
       </c>

</xml_diff>

<commit_message>
Descripción de los cambios, Actualizar precios.
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="424">
   <si>
     <t>Nombre</t>
   </si>
@@ -1290,6 +1290,15 @@
   </si>
   <si>
     <t>Ventilador Cuello Portátil 5 Modos Usb Recargable Silencioso</t>
+  </si>
+  <si>
+    <t>https://articulo.mercadolibre.com.mx/MLM-2198847593-ventilador-cuello-portatil-5-modos-usb-recargable-silencioso-_JM?quantity=1&amp;variation_id=186278346493</t>
+  </si>
+  <si>
+    <t>https://http2.mlstatic.com/D_685542-MLM83342993232_042025-N.jpg</t>
+  </si>
+  <si>
+    <t>https://http2.mlstatic.com/D_NQ_NP_2X_998777-MLM54133192046_032023-F-mini-aire-acondicionado-portatil-enfriador-clima-escritorio.webp</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1791,7 @@
   <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,7 +1937,9 @@
       <c r="D7" s="4">
         <v>150</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>423</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>419</v>
       </c>
@@ -1963,8 +1974,12 @@
       <c r="D9" s="4">
         <v>180</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5164,11 +5179,14 @@
     <hyperlink ref="F15"/>
     <hyperlink ref="E15" r:id="rId243"/>
     <hyperlink ref="F7" r:id="rId244"/>
+    <hyperlink ref="F9" r:id="rId245"/>
+    <hyperlink ref="E9" r:id="rId246"/>
+    <hyperlink ref="E7" r:id="rId247"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId245"/>
+  <pageSetup orientation="portrait" r:id="rId248"/>
   <tableParts count="1">
-    <tablePart r:id="rId246"/>
+    <tablePart r:id="rId249"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Descripción de los cambios 03012026
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -2054,15 +2054,23 @@
     <t>https://http2.mlstatic.com/D_NQ_NP_2X_973202-MLM98639006023_112025-F-lijadora-orbital-electrica-360w-14000rpm-con-6-velocidades.webp</t>
   </si>
   <si>
-    <t>https://scontent.fcul3-1.fna.fbcdn.net/v/t45.5328-4/578855730_1355716606260688_6335837657304903512_n.jpg?stp=dst-jpg_p960x960_tt6&amp;_nc_cat=107&amp;ccb=1-7&amp;_nc_sid=247b10&amp;_nc_ohc=e-nWx9D9jTcQ7kNvwGI5bN7&amp;_nc_oc=Adl1OTv5o5eolm07FKKKEOWN0lViSHNFCj2xIlpyzKVAxbku7UEhEKenjEiJJlV5Bsk&amp;_nc_zt=23&amp;_nc_ht=scontent.fcul3-1.fna&amp;_nc_gid=jiAvmZSigUPnLZg3QOd2Vw&amp;oh=00_Afr3mW5amgn7B42rHImZMsKX6wHL7bAGdMUHCGuV15PvaA&amp;oe=695F9CA7</t>
+    <t>https://charming-panda-45bed1.netlify.app/imagenes/578855730_1355716606260688_6335837657304903512_n.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2096,7 +2104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2105,6 +2113,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2411,7 +2420,7 @@
   <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5438,8 +5447,8 @@
       <c r="C136">
         <v>1050</v>
       </c>
-      <c r="D136">
-        <v>550</v>
+      <c r="D136" s="4">
+        <v>600</v>
       </c>
       <c r="E136" t="s">
         <v>674</v>
@@ -6919,8 +6928,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>